<commit_message>
add cuda and pandas
</commit_message>
<xml_diff>
--- a/pandas/cs401_out.xlsx
+++ b/pandas/cs401_out.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="advisors" sheetId="2" r:id="rId2"/>
+    <sheet name="date" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="262">
   <si>
     <t>Timestamp</t>
   </si>
@@ -41,171 +42,6 @@
     <t>อาจารย์ที่ปรึกษาโครงงาน</t>
   </si>
   <si>
-    <t>8/24/2015 13:06:02</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:11:03</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:11:32</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:13:33</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:14:14</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:14:16</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:14:31</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:15:28</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:15:35</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:15:44</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:16:56</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:16:58</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:19:36</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:20:10</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:20:13</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:22:36</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:22:51</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:23:47</t>
-  </si>
-  <si>
-    <t>8/24/2015 13:26:41</t>
-  </si>
-  <si>
-    <t>8/24/2015 14:04:20</t>
-  </si>
-  <si>
-    <t>8/24/2015 15:32:24</t>
-  </si>
-  <si>
-    <t>8/24/2015 19:57:21</t>
-  </si>
-  <si>
-    <t>8/24/2015 20:13:18</t>
-  </si>
-  <si>
-    <t>8/24/2015 21:32:36</t>
-  </si>
-  <si>
-    <t>8/24/2015 22:41:05</t>
-  </si>
-  <si>
-    <t>8/24/2015 23:37:39</t>
-  </si>
-  <si>
-    <t>8/25/2015 1:16:02</t>
-  </si>
-  <si>
-    <t>8/25/2015 7:48:39</t>
-  </si>
-  <si>
-    <t>8/25/2015 10:12:25</t>
-  </si>
-  <si>
-    <t>8/25/2015 11:19:24</t>
-  </si>
-  <si>
-    <t>8/25/2015 14:10:13</t>
-  </si>
-  <si>
-    <t>8/25/2015 16:48:48</t>
-  </si>
-  <si>
-    <t>8/26/2015 11:38:36</t>
-  </si>
-  <si>
-    <t>8/26/2015 14:12:59</t>
-  </si>
-  <si>
-    <t>8/26/2015 22:23:53</t>
-  </si>
-  <si>
-    <t>8/27/2015 12:55:23</t>
-  </si>
-  <si>
-    <t>8/27/2015 21:42:41</t>
-  </si>
-  <si>
-    <t>8/28/2015 0:22:40</t>
-  </si>
-  <si>
-    <t>8/28/2015 0:36:42</t>
-  </si>
-  <si>
-    <t>8/28/2015 21:57:43</t>
-  </si>
-  <si>
-    <t>8/29/2015 8:57:29</t>
-  </si>
-  <si>
-    <t>8/31/2015 12:43:49</t>
-  </si>
-  <si>
-    <t>8/31/2015 19:52:47</t>
-  </si>
-  <si>
-    <t>9/2/2015 0:41:33</t>
-  </si>
-  <si>
-    <t>9/3/2015 9:44:49</t>
-  </si>
-  <si>
-    <t>9/3/2015 20:36:50</t>
-  </si>
-  <si>
-    <t>9/5/2015 11:30:31</t>
-  </si>
-  <si>
-    <t>9/5/2015 11:30:51</t>
-  </si>
-  <si>
-    <t>9/6/2015 1:47:23</t>
-  </si>
-  <si>
-    <t>9/6/2015 21:35:15</t>
-  </si>
-  <si>
-    <t>9/7/2015 10:01:07</t>
-  </si>
-  <si>
-    <t>9/9/2015 17:56:32</t>
-  </si>
-  <si>
-    <t>9/14/2015 9:42:53</t>
-  </si>
-  <si>
-    <t>9/14/2015 9:58:08</t>
-  </si>
-  <si>
-    <t>9/14/2015 14:04:09</t>
-  </si>
-  <si>
     <t>นางสาว พัทธนันทร์ อนันต์เจริญภากร</t>
   </si>
   <si>
@@ -251,7 +87,7 @@
     <t>ลดาวัลย์ สรรพโส</t>
   </si>
   <si>
-    <t>ภรารัตน์  ตันติประภากิจ</t>
+    <t>กนภา ตระกูลวรรณชัย</t>
   </si>
   <si>
     <t>วทัญญู ภารตรัตน์</t>
@@ -284,7 +120,7 @@
     <t>นางสาวกชกร เมธาวี</t>
   </si>
   <si>
-    <t>นาย ธนภัทร สังข์กระแสร์</t>
+    <t>ธนภัทร สังข์กระแสร์</t>
   </si>
   <si>
     <t>นางสาวปิยะพร ใจเอื้อย</t>
@@ -305,9 +141,6 @@
     <t>พันธวิศ เจริญผล</t>
   </si>
   <si>
-    <t>ภรณ์หทัย ถนอมวงษ์</t>
-  </si>
-  <si>
     <t>กันตวีร์ วรชื่น</t>
   </si>
   <si>
@@ -320,7 +153,7 @@
     <t>คุณภัทร แสนดวงดี</t>
   </si>
   <si>
-    <t>อติชาติ สิินส่งสุข</t>
+    <t>อติชาติ สินส่งสุข</t>
   </si>
   <si>
     <t>สุรวัช อำพัน</t>
@@ -368,6 +201,21 @@
     <t>เตชิต ยิ่งยงชัย</t>
   </si>
   <si>
+    <t>ธนพล ขจรกลิ่นมาลา</t>
+  </si>
+  <si>
+    <t>นายกฤตนนท์ เงินเจริญ</t>
+  </si>
+  <si>
+    <t>จิรายุ อิงคสุวรรณศิริ</t>
+  </si>
+  <si>
+    <t>ทัตพล พูลอำไภย์</t>
+  </si>
+  <si>
+    <t>พิมพ์ชนก หรูเจริญพงษ์</t>
+  </si>
+  <si>
     <t>นาย พงศธร ลิมป์กาญจนวัฒน์</t>
   </si>
   <si>
@@ -401,9 +249,6 @@
     <t>ปริญญา อ่อนสุวรรณ์</t>
   </si>
   <si>
-    <t>กนภา  ตระกูลวรรณชัย</t>
-  </si>
-  <si>
     <t>วรากร รักรอด</t>
   </si>
   <si>
@@ -449,9 +294,6 @@
     <t>ฆนาพงศ์ โพธิ์ทอง</t>
   </si>
   <si>
-    <t>ณิชาภัทร สิงขรอาจ</t>
-  </si>
-  <si>
     <t>สุรัชนี แจ้งศิลป์</t>
   </si>
   <si>
@@ -491,9 +333,24 @@
     <t>น.ส.ภรณ์หทัย  ถนอมวงษ์</t>
   </si>
   <si>
+    <t>พิมพกานต์ วรรณศิริกุล</t>
+  </si>
+  <si>
+    <t>ปรเมศวร์ หอมนาน</t>
+  </si>
+  <si>
+    <t>สาคเรศ ยงไพศาลทรัพย์</t>
+  </si>
+  <si>
     <t>ชิตะ สิรยาทร</t>
   </si>
   <si>
+    <t>ภรารัตน์ ตันติประภากิจ</t>
+  </si>
+  <si>
+    <t>สักการ หลลักเพชร์</t>
+  </si>
+  <si>
     <t>อาจารย์ นุชชากร งามเสาวรส</t>
   </si>
   <si>
@@ -567,12 +424,459 @@
   </si>
   <si>
     <t>special</t>
+  </si>
+  <si>
+    <t>01วันที่ [8	เช้า]</t>
+  </si>
+  <si>
+    <t>02วันที่ [8	บ่าย]</t>
+  </si>
+  <si>
+    <t>03วันที่ [9	เช้า]</t>
+  </si>
+  <si>
+    <t>04วันที่ [9	บ่าย]</t>
+  </si>
+  <si>
+    <t>05วันที่ [10	เช้า]</t>
+  </si>
+  <si>
+    <t>06วันที่ [10	บ่าย]</t>
+  </si>
+  <si>
+    <t>07วันที่ [11	เช้า]</t>
+  </si>
+  <si>
+    <t>08วันที่ [11	บ่าย]</t>
+  </si>
+  <si>
+    <t>09วันที่ [12	เช้า]</t>
+  </si>
+  <si>
+    <t>10วันที่ [12	บ่าย]</t>
+  </si>
+  <si>
+    <t>11วันที่ [13	เช้า]</t>
+  </si>
+  <si>
+    <t>12วันที่ [13	บ่าย]</t>
+  </si>
+  <si>
+    <t>13วันที่ [14	เช้า]</t>
+  </si>
+  <si>
+    <t>14วันที่ [14	บ่าย]</t>
+  </si>
+  <si>
+    <t>15วันที่ [15	เช้า]</t>
+  </si>
+  <si>
+    <t>16วันที่ [15	บ่าย]</t>
+  </si>
+  <si>
+    <t>17วันที่ [16	เช้า]</t>
+  </si>
+  <si>
+    <t>18วันที่ [16	บ่าย]</t>
+  </si>
+  <si>
+    <t>19วันที่ [17	เช้า]</t>
+  </si>
+  <si>
+    <t>20วันที่ [17	บ่าย]</t>
+  </si>
+  <si>
+    <t>21วันที่ [18	เช้า]</t>
+  </si>
+  <si>
+    <t>22วันที่ [18	บ่าย]</t>
+  </si>
+  <si>
+    <t>23วันที่ [19	เช้า]</t>
+  </si>
+  <si>
+    <t>24วันที่ [19	บ่าย]</t>
+  </si>
+  <si>
+    <t>25วันที่ [20	เช้า]</t>
+  </si>
+  <si>
+    <t>26วันที่ [20	บ่าย]</t>
+  </si>
+  <si>
+    <t>27วันที่ [21	เช้า]</t>
+  </si>
+  <si>
+    <t>28วันที่ [21	บ่าย]</t>
+  </si>
+  <si>
+    <t>29วันที่ [22	เช้า]</t>
+  </si>
+  <si>
+    <t>30วันที่ [22	บ่าย]</t>
+  </si>
+  <si>
+    <t>31วันที่ [23	เช้า]</t>
+  </si>
+  <si>
+    <t>32วันที่ [23	บ่าย]</t>
+  </si>
+  <si>
+    <t>33วันที่ [24	เช้า]</t>
+  </si>
+  <si>
+    <t>34วันที่ [24	บ่าย]</t>
+  </si>
+  <si>
+    <t>35วันที่ [25	เช้า]</t>
+  </si>
+  <si>
+    <t>36วันที่ [25	บ่าย]</t>
+  </si>
+  <si>
+    <t>37วันที่ [26	เช้า]</t>
+  </si>
+  <si>
+    <t>38วันที่ [26	บ่าย]</t>
+  </si>
+  <si>
+    <t>39วันที่ [27	เช้า]</t>
+  </si>
+  <si>
+    <t>40วันที่ [27	บ่าย]</t>
+  </si>
+  <si>
+    <t>41วันที่ [28	เช้า]</t>
+  </si>
+  <si>
+    <t>42วันที่ [28	บ่าย]</t>
+  </si>
+  <si>
+    <t>5509620026
+5509611801
+5509611579
+5509650700</t>
+  </si>
+  <si>
+    <t>5509611553
+5509612023</t>
+  </si>
+  <si>
+    <t>5509530019</t>
+  </si>
+  <si>
+    <t>5509611975
+5509450010</t>
+  </si>
+  <si>
+    <t>5509611843</t>
+  </si>
+  <si>
+    <t>5509611512</t>
+  </si>
+  <si>
+    <t>5509611538
+5509612072</t>
+  </si>
+  <si>
+    <t>5509611785</t>
+  </si>
+  <si>
+    <t>5509650296</t>
+  </si>
+  <si>
+    <t>5509650106
+5509650700</t>
+  </si>
+  <si>
+    <t>5509650700</t>
+  </si>
+  <si>
+    <t>5509611702
+5509620026
+5509611801
+5509650387</t>
+  </si>
+  <si>
+    <t>5509611553</t>
+  </si>
+  <si>
+    <t>5509611561
+5509611652</t>
+  </si>
+  <si>
+    <t>5509611819
+5509650635</t>
+  </si>
+  <si>
+    <t>5509650247
+5509650577
+5509450010</t>
+  </si>
+  <si>
+    <t>5509650825</t>
+  </si>
+  <si>
+    <t>5509650569</t>
+  </si>
+  <si>
+    <t>5509650171
+5509650429</t>
+  </si>
+  <si>
+    <t>5509611702
+5509650700</t>
+  </si>
+  <si>
+    <t>5509611587</t>
+  </si>
+  <si>
+    <t>5509650254</t>
+  </si>
+  <si>
+    <t>5509611538</t>
+  </si>
+  <si>
+    <t>5509650171</t>
+  </si>
+  <si>
+    <t>5509650916</t>
+  </si>
+  <si>
+    <t>5509650221
+5509650221
+5509650106
+5509611579
+5509650387</t>
+  </si>
+  <si>
+    <t>5509650254
+5509650445</t>
+  </si>
+  <si>
+    <t>5509650650</t>
+  </si>
+  <si>
+    <t>5509650783</t>
+  </si>
+  <si>
+    <t>5509520044</t>
+  </si>
+  <si>
+    <t>5509611868</t>
+  </si>
+  <si>
+    <t>5509650627
+5509650809</t>
+  </si>
+  <si>
+    <t>5509680061
+5509611637</t>
+  </si>
+  <si>
+    <t>5509611975
+5509650247</t>
+  </si>
+  <si>
+    <t>5509490016</t>
+  </si>
+  <si>
+    <t>5509650619</t>
+  </si>
+  <si>
+    <t>5509611785
+5509611736</t>
+  </si>
+  <si>
+    <t>5509650932
+5509611454</t>
+  </si>
+  <si>
+    <t>5509650544</t>
+  </si>
+  <si>
+    <t>5509620026
+5509611801</t>
+  </si>
+  <si>
+    <t>5509612122
+5509650254</t>
+  </si>
+  <si>
+    <t>5509650270
+5509650270</t>
+  </si>
+  <si>
+    <t>5509520051</t>
+  </si>
+  <si>
+    <t>5509650031
+5509650247
+5509650502</t>
+  </si>
+  <si>
+    <t>5509650239</t>
+  </si>
+  <si>
+    <t>5309610078
+5509650171
+5509650429</t>
+  </si>
+  <si>
+    <t>5509611454</t>
+  </si>
+  <si>
+    <t>5509650221
+5509650221
+5509650106
+5509620026
+5509611801
+5509611579</t>
+  </si>
+  <si>
+    <t>5509612122
+5509650254
+5509650445</t>
+  </si>
+  <si>
+    <t>5509611611</t>
+  </si>
+  <si>
+    <t>5509650635
+5509650544</t>
+  </si>
+  <si>
+    <t>5509611496
+5509680061
+5509611637</t>
+  </si>
+  <si>
+    <t>5509611975</t>
+  </si>
+  <si>
+    <t>5509490016
+5509612031
+5509612031</t>
+  </si>
+  <si>
+    <t>5509611538
+5509612072
+5509650460
+5509650825</t>
+  </si>
+  <si>
+    <t>5509650429</t>
+  </si>
+  <si>
+    <t>5509650916
+5509650932</t>
+  </si>
+  <si>
+    <t>5509650221
+5509650221
+5509650106</t>
+  </si>
+  <si>
+    <t>5509611496</t>
+  </si>
+  <si>
+    <t>5509650577</t>
+  </si>
+  <si>
+    <t>5509612031
+5509612031</t>
+  </si>
+  <si>
+    <t>5509611801
+5509611579
+5509650387</t>
+  </si>
+  <si>
+    <t>5509650445</t>
+  </si>
+  <si>
+    <t>5509611561</t>
+  </si>
+  <si>
+    <t>5509611868
+5509650544</t>
+  </si>
+  <si>
+    <t>5509650627</t>
+  </si>
+  <si>
+    <t>5509612023</t>
+  </si>
+  <si>
+    <t>5509612072</t>
+  </si>
+  <si>
+    <t>5509611561
+5509611652
+5509650270
+5509650270</t>
+  </si>
+  <si>
+    <t>5509611884
+5509611603</t>
+  </si>
+  <si>
+    <t>5509611819
+5509650544</t>
+  </si>
+  <si>
+    <t>5509611587
+5509611900
+5509611975
+5509650577
+5509450010</t>
+  </si>
+  <si>
+    <t>5509650932</t>
+  </si>
+  <si>
+    <t>5509611702</t>
+  </si>
+  <si>
+    <t>5509620026</t>
+  </si>
+  <si>
+    <t>5509612122</t>
+  </si>
+  <si>
+    <t>5509611603</t>
+  </si>
+  <si>
+    <t>5509650460</t>
+  </si>
+  <si>
+    <t>5509611827
+5509612106</t>
+  </si>
+  <si>
+    <t>5509450010</t>
+  </si>
+  <si>
+    <t>5509650734
+5509650825</t>
+  </si>
+  <si>
+    <t>5509650163</t>
+  </si>
+  <si>
+    <t>5509650734</t>
+  </si>
+  <si>
+    <t>5509611736</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -625,11 +929,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,7 +1229,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -960,8 +1265,8 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
+      <c r="B2" s="2">
+        <v>42240.5458566551</v>
       </c>
       <c r="C2">
         <v>5509611785</v>
@@ -970,21 +1275,21 @@
         <v>5509611629</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
+      <c r="B3" s="2">
+        <v>42240.5493439005</v>
       </c>
       <c r="C3">
         <v>5509650031</v>
@@ -993,21 +1298,21 @@
         <v>5509650502</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="I3" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
+      <c r="B4" s="2">
+        <v>42240.5496806018</v>
       </c>
       <c r="C4">
         <v>5509650494</v>
@@ -1016,38 +1321,38 @@
         <v>5509650379</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="I4" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
+      <c r="B5" s="2">
+        <v>42240.5510754051</v>
       </c>
       <c r="C5">
         <v>5509650700</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
+      <c r="B6" s="2">
+        <v>42240.5515458681</v>
       </c>
       <c r="C6">
         <v>5509611769</v>
@@ -1056,38 +1361,38 @@
         <v>5509611850</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
+      <c r="B7" s="2">
+        <v>42240.5515720833</v>
       </c>
       <c r="C7">
         <v>5509680038</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="I7" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
+      <c r="B8" s="2">
+        <v>42240.5517500232</v>
       </c>
       <c r="C8">
         <v>5509611975</v>
@@ -1096,55 +1401,55 @@
         <v>5509611900</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="I8" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
+      <c r="B9" s="2">
+        <v>42240.5524123148</v>
       </c>
       <c r="C9">
         <v>5509611520</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
+      <c r="B10" s="2">
+        <v>42240.5524868981</v>
       </c>
       <c r="C10">
         <v>5509650734</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
+      <c r="B11" s="2">
+        <v>42240.5525956019</v>
       </c>
       <c r="C11">
         <v>5509611694</v>
@@ -1153,21 +1458,21 @@
         <v>5509611702</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>18</v>
+      <c r="B12" s="2">
+        <v>42240.5534287384</v>
       </c>
       <c r="C12">
         <v>5409650453</v>
@@ -1179,24 +1484,24 @@
         <v>5509650569</v>
       </c>
       <c r="F12" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="H12" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="I12" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
+      <c r="B13" s="2">
+        <v>42240.5534458102</v>
       </c>
       <c r="C13">
         <v>5509650239</v>
@@ -1205,21 +1510,21 @@
         <v>5509650452</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>165</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>20</v>
+      <c r="B14" s="2">
+        <v>42240.5552769676</v>
       </c>
       <c r="C14">
         <v>5509680012</v>
@@ -1228,21 +1533,21 @@
         <v>5509680053</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="G14" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>21</v>
+      <c r="B15" s="2">
+        <v>42240.5556756018</v>
       </c>
       <c r="C15">
         <v>5509611561</v>
@@ -1251,21 +1556,21 @@
         <v>5509611652</v>
       </c>
       <c r="F15" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="I15" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>22</v>
+      <c r="B16" s="2">
+        <v>42240.555708287</v>
       </c>
       <c r="C16">
         <v>5509650247</v>
@@ -1274,44 +1579,38 @@
         <v>5509650577</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2">
+        <v>42240.5573668056</v>
+      </c>
+      <c r="C17">
+        <v>5509650528</v>
+      </c>
+      <c r="F17" t="s">
         <v>23</v>
       </c>
-      <c r="C17">
-        <v>5509650621</v>
-      </c>
-      <c r="D17">
-        <v>5509650528</v>
-      </c>
-      <c r="F17" t="s">
-        <v>78</v>
-      </c>
-      <c r="G17" t="s">
-        <v>128</v>
-      </c>
       <c r="I17" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>24</v>
+      <c r="B18" s="2">
+        <v>42240.5575310764</v>
       </c>
       <c r="C18">
         <v>5509530019</v>
@@ -1320,21 +1619,21 @@
         <v>5509611488</v>
       </c>
       <c r="F18" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="I18" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>25</v>
+      <c r="B19" s="2">
+        <v>42240.5581771875</v>
       </c>
       <c r="C19">
         <v>5509650106</v>
@@ -1342,22 +1641,28 @@
       <c r="D19">
         <v>5509650387</v>
       </c>
+      <c r="E19">
+        <v>5509650221</v>
+      </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>130</v>
+        <v>78</v>
+      </c>
+      <c r="H19" t="s">
+        <v>109</v>
       </c>
       <c r="I19" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>26</v>
+      <c r="B20" s="2">
+        <v>42240.560195706</v>
       </c>
       <c r="C20">
         <v>5509611736</v>
@@ -1366,21 +1671,21 @@
         <v>5509611744</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="I20" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>27</v>
+      <c r="B21" s="2">
+        <v>42240.5863472917</v>
       </c>
       <c r="C21">
         <v>5509450010</v>
@@ -1389,21 +1694,21 @@
         <v>5509611587</v>
       </c>
       <c r="F21" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="G21" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="I21" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>28</v>
+      <c r="B22" s="2">
+        <v>42240.6474988542</v>
       </c>
       <c r="C22">
         <v>5509611637</v>
@@ -1412,21 +1717,21 @@
         <v>5509680061</v>
       </c>
       <c r="F22" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="G22" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="I22" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>29</v>
+      <c r="B23" s="2">
+        <v>42240.8314943056</v>
       </c>
       <c r="C23">
         <v>5509611538</v>
@@ -1435,21 +1740,21 @@
         <v>5509612072</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="G23" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="I23" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>30</v>
+      <c r="B24" s="2">
+        <v>42240.8425742014</v>
       </c>
       <c r="C24">
         <v>5509650171</v>
@@ -1458,21 +1763,21 @@
         <v>5509650429</v>
       </c>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
       <c r="I24" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>31</v>
+      <c r="B25" s="2">
+        <v>42240.8976350347</v>
       </c>
       <c r="C25">
         <v>5509650296</v>
@@ -1481,38 +1786,38 @@
         <v>5709611692</v>
       </c>
       <c r="F25" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="G25" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="I25" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>32</v>
+      <c r="B26" s="2">
+        <v>42240.9451917245</v>
       </c>
       <c r="C26">
         <v>5509520028</v>
       </c>
       <c r="F26" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="I26" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>33</v>
+      <c r="B27" s="2">
+        <v>42240.9844810185</v>
       </c>
       <c r="C27">
         <v>5509611777</v>
@@ -1521,38 +1826,38 @@
         <v>5509611835</v>
       </c>
       <c r="F27" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="G27" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="I27" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>34</v>
+      <c r="B28" s="2">
+        <v>42241.0528021759</v>
       </c>
       <c r="C28">
         <v>5509612114</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="I28" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>35</v>
+      <c r="B29" s="2">
+        <v>42241.3254525463</v>
       </c>
       <c r="C29">
         <v>5509520044</v>
@@ -1561,21 +1866,21 @@
         <v>5509680046</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="G29" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="I29" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>36</v>
+      <c r="B30" s="2">
+        <v>42241.4252893403</v>
       </c>
       <c r="C30">
         <v>5509611801</v>
@@ -1584,21 +1889,21 @@
         <v>5509620026</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="G30" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="I30" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>37</v>
+      <c r="B31" s="2">
+        <v>42241.4717998264</v>
       </c>
       <c r="C31">
         <v>5509611827</v>
@@ -1607,21 +1912,21 @@
         <v>5509612106</v>
       </c>
       <c r="F31" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="G31" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="I31" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>38</v>
+      <c r="B32" s="2">
+        <v>42241.5904246065</v>
       </c>
       <c r="C32">
         <v>5509650627</v>
@@ -1630,21 +1935,21 @@
         <v>5509650809</v>
       </c>
       <c r="F32" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="G32" t="s">
-        <v>141</v>
+        <v>89</v>
       </c>
       <c r="I32" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
-        <v>39</v>
+      <c r="B33" s="2">
+        <v>42241.7005609144</v>
       </c>
       <c r="C33">
         <v>5509490016</v>
@@ -1653,21 +1958,21 @@
         <v>5509612031</v>
       </c>
       <c r="F33" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="G33" t="s">
-        <v>142</v>
+        <v>90</v>
       </c>
       <c r="I33" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>40</v>
+      <c r="B34" s="2">
+        <v>42242.4851408912</v>
       </c>
       <c r="C34">
         <v>5509650635</v>
@@ -1676,477 +1981,551 @@
         <v>5509650163</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="I34" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2">
+        <v>42242.9332561806</v>
+      </c>
+      <c r="C35">
+        <v>5509611611</v>
+      </c>
+      <c r="F35" t="s">
         <v>41</v>
       </c>
-      <c r="C35">
-        <v>5509650270</v>
-      </c>
-      <c r="D35">
-        <v>5509650353</v>
-      </c>
-      <c r="F35" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" t="s">
-        <v>144</v>
-      </c>
       <c r="I35" t="s">
-        <v>167</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="2">
+        <v>42243.5384583565</v>
+      </c>
+      <c r="C36">
+        <v>5509611819</v>
+      </c>
+      <c r="D36">
+        <v>5509611868</v>
+      </c>
+      <c r="F36" t="s">
         <v>42</v>
       </c>
-      <c r="C36">
-        <v>5509611611</v>
-      </c>
-      <c r="F36" t="s">
-        <v>97</v>
+      <c r="G36" t="s">
+        <v>92</v>
       </c>
       <c r="I36" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2">
+        <v>42243.9046469676</v>
+      </c>
+      <c r="C37">
+        <v>5509650916</v>
+      </c>
+      <c r="D37">
+        <v>5509650932</v>
+      </c>
+      <c r="F37" t="s">
         <v>43</v>
       </c>
-      <c r="C37">
-        <v>5509611819</v>
-      </c>
-      <c r="D37">
-        <v>5509611868</v>
-      </c>
-      <c r="F37" t="s">
-        <v>98</v>
-      </c>
       <c r="G37" t="s">
-        <v>145</v>
+        <v>93</v>
       </c>
       <c r="I37" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="2">
+        <v>42244.0157437616</v>
+      </c>
+      <c r="C38">
+        <v>5509611553</v>
+      </c>
+      <c r="D38">
+        <v>5509612023</v>
+      </c>
+      <c r="F38" t="s">
         <v>44</v>
       </c>
-      <c r="C38">
-        <v>5509650916</v>
-      </c>
-      <c r="D38">
-        <v>5509650932</v>
-      </c>
-      <c r="F38" t="s">
-        <v>99</v>
-      </c>
       <c r="G38" t="s">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="I38" t="s">
-        <v>175</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2">
+        <v>42244.0254809028</v>
+      </c>
+      <c r="C39">
+        <v>5509611512</v>
+      </c>
+      <c r="F39" t="s">
         <v>45</v>
       </c>
-      <c r="C39">
-        <v>5509611553</v>
-      </c>
-      <c r="D39">
-        <v>5509612023</v>
-      </c>
-      <c r="F39" t="s">
-        <v>100</v>
-      </c>
-      <c r="G39" t="s">
-        <v>147</v>
-      </c>
       <c r="I39" t="s">
-        <v>176</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="2">
+        <v>42244.9150775231</v>
+      </c>
+      <c r="C40">
+        <v>5509650544</v>
+      </c>
+      <c r="F40" t="s">
         <v>46</v>
       </c>
-      <c r="C40">
-        <v>5509611512</v>
-      </c>
-      <c r="F40" t="s">
-        <v>101</v>
-      </c>
       <c r="I40" t="s">
-        <v>173</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2">
+        <v>42245.3732568287</v>
+      </c>
+      <c r="C41">
+        <v>5409650115</v>
+      </c>
+      <c r="F41" t="s">
         <v>47</v>
       </c>
-      <c r="C41">
-        <v>5509650544</v>
-      </c>
-      <c r="F41" t="s">
-        <v>102</v>
-      </c>
       <c r="I41" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2">
+        <v>42247.5304288079</v>
+      </c>
+      <c r="C42">
+        <v>5509611496</v>
+      </c>
+      <c r="D42">
+        <v>5509611546</v>
+      </c>
+      <c r="F42" t="s">
         <v>48</v>
       </c>
-      <c r="C42">
-        <v>5409650115</v>
-      </c>
-      <c r="F42" t="s">
-        <v>103</v>
+      <c r="G42" t="s">
+        <v>95</v>
       </c>
       <c r="I42" t="s">
-        <v>175</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2">
+        <v>42247.8283174306</v>
+      </c>
+      <c r="C43">
+        <v>5509611454</v>
+      </c>
+      <c r="F43" t="s">
         <v>49</v>
       </c>
-      <c r="C43">
-        <v>5509611496</v>
-      </c>
-      <c r="D43">
-        <v>5509611546</v>
-      </c>
-      <c r="F43" t="s">
-        <v>104</v>
-      </c>
-      <c r="G43" t="s">
-        <v>148</v>
-      </c>
       <c r="I43" t="s">
-        <v>168</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2">
+        <v>42249.0288551852</v>
+      </c>
+      <c r="C44">
+        <v>5509650783</v>
+      </c>
+      <c r="F44" t="s">
         <v>50</v>
       </c>
-      <c r="C44">
-        <v>5509611454</v>
-      </c>
-      <c r="F44" t="s">
-        <v>105</v>
-      </c>
       <c r="I44" t="s">
-        <v>175</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2">
+        <v>42250.4061212963</v>
+      </c>
+      <c r="C45">
+        <v>5509611603</v>
+      </c>
+      <c r="D45">
+        <v>5509611884</v>
+      </c>
+      <c r="F45" t="s">
         <v>51</v>
       </c>
-      <c r="C45">
-        <v>5509650783</v>
-      </c>
-      <c r="F45" t="s">
-        <v>106</v>
+      <c r="G45" t="s">
+        <v>96</v>
       </c>
       <c r="I45" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2">
+        <v>42250.8589063889</v>
+      </c>
+      <c r="C46">
+        <v>5509650254</v>
+      </c>
+      <c r="D46">
+        <v>5509612122</v>
+      </c>
+      <c r="F46" t="s">
         <v>52</v>
       </c>
-      <c r="C46">
-        <v>5509611603</v>
-      </c>
-      <c r="D46">
-        <v>5509611884</v>
-      </c>
-      <c r="F46" t="s">
-        <v>107</v>
-      </c>
       <c r="G46" t="s">
-        <v>149</v>
+        <v>97</v>
       </c>
       <c r="I46" t="s">
-        <v>177</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2">
+        <v>42252.4797542245</v>
+      </c>
+      <c r="C47">
+        <v>5509650650</v>
+      </c>
+      <c r="D47">
+        <v>5509650676</v>
+      </c>
+      <c r="F47" t="s">
         <v>53</v>
       </c>
-      <c r="C47">
-        <v>5509650254</v>
-      </c>
-      <c r="D47">
-        <v>5509612122</v>
-      </c>
-      <c r="F47" t="s">
-        <v>108</v>
-      </c>
       <c r="G47" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="I47" t="s">
-        <v>178</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="2">
+        <v>42253.0745702894</v>
+      </c>
+      <c r="C48">
+        <v>5509611595</v>
+      </c>
+      <c r="D48">
+        <v>5509611967</v>
+      </c>
+      <c r="F48" t="s">
         <v>54</v>
       </c>
-      <c r="C48">
-        <v>5509650650</v>
-      </c>
-      <c r="D48">
-        <v>5509650676</v>
-      </c>
-      <c r="F48" t="s">
-        <v>109</v>
-      </c>
       <c r="G48" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
       <c r="I48" t="s">
-        <v>179</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2">
+        <v>42253.899478044</v>
+      </c>
+      <c r="C49">
+        <v>5509611843</v>
+      </c>
+      <c r="D49">
+        <v>5509611942</v>
+      </c>
+      <c r="F49" t="s">
         <v>55</v>
       </c>
-      <c r="C49">
-        <v>5509650650</v>
-      </c>
-      <c r="D49">
-        <v>5509650676</v>
-      </c>
-      <c r="F49" t="s">
-        <v>109</v>
-      </c>
       <c r="G49" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="I49" t="s">
-        <v>179</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="2">
+        <v>42254.4174381366</v>
+      </c>
+      <c r="C50">
+        <v>5509650825</v>
+      </c>
+      <c r="D50">
+        <v>5509650619</v>
+      </c>
+      <c r="F50" t="s">
         <v>56</v>
       </c>
-      <c r="C50">
-        <v>5509611595</v>
-      </c>
-      <c r="D50">
-        <v>5509611967</v>
-      </c>
-      <c r="F50" t="s">
-        <v>110</v>
-      </c>
       <c r="G50" t="s">
-        <v>152</v>
+        <v>101</v>
       </c>
       <c r="I50" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2">
+        <v>42256.7475893287</v>
+      </c>
+      <c r="C51">
+        <v>5509650312</v>
+      </c>
+      <c r="D51">
+        <v>5509650445</v>
+      </c>
+      <c r="F51" t="s">
         <v>57</v>
       </c>
-      <c r="C51">
-        <v>5509611843</v>
-      </c>
-      <c r="D51">
-        <v>5509611942</v>
-      </c>
-      <c r="F51" t="s">
-        <v>111</v>
-      </c>
       <c r="G51" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
       <c r="I51" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="2">
+        <v>42261.4047762963</v>
+      </c>
+      <c r="C52">
+        <v>5509650585</v>
+      </c>
+      <c r="D52">
+        <v>5509650684</v>
+      </c>
+      <c r="F52" t="s">
         <v>58</v>
       </c>
-      <c r="C52">
-        <v>5509650825</v>
-      </c>
-      <c r="D52">
-        <v>5509650619</v>
-      </c>
-      <c r="F52" t="s">
-        <v>112</v>
-      </c>
       <c r="G52" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
       <c r="I52" t="s">
-        <v>164</v>
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2">
+        <v>42261.4153751505</v>
+      </c>
+      <c r="C53">
+        <v>5509650353</v>
+      </c>
+      <c r="D53">
+        <v>5509650270</v>
+      </c>
+      <c r="F53" t="s">
         <v>59</v>
       </c>
-      <c r="C53">
-        <v>5509650312</v>
-      </c>
-      <c r="D53">
-        <v>5509650445</v>
-      </c>
-      <c r="F53" t="s">
-        <v>113</v>
-      </c>
       <c r="G53" t="s">
-        <v>155</v>
+        <v>104</v>
       </c>
       <c r="I53" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2">
+        <v>42261.5862134838</v>
+      </c>
+      <c r="C54">
+        <v>5509650478</v>
+      </c>
+      <c r="F54" t="s">
         <v>60</v>
       </c>
-      <c r="C54">
-        <v>5509650585</v>
-      </c>
-      <c r="D54">
-        <v>5509650684</v>
-      </c>
-      <c r="F54" t="s">
-        <v>114</v>
-      </c>
-      <c r="G54" t="s">
-        <v>156</v>
-      </c>
       <c r="I54" t="s">
-        <v>179</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2">
+        <v>42269.9708474421</v>
+      </c>
+      <c r="C55">
+        <v>5509611918</v>
+      </c>
+      <c r="D55">
+        <v>5509611579</v>
+      </c>
+      <c r="F55" t="s">
         <v>61</v>
       </c>
-      <c r="C55">
-        <v>5509650353</v>
-      </c>
-      <c r="D55">
-        <v>5509650270</v>
-      </c>
-      <c r="F55" t="s">
-        <v>115</v>
-      </c>
       <c r="G55" t="s">
-        <v>157</v>
+        <v>105</v>
       </c>
       <c r="I55" t="s">
-        <v>167</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="2">
+        <v>42272.9150974653</v>
+      </c>
+      <c r="C56">
+        <v>5509520051</v>
+      </c>
+      <c r="H56" t="s">
+        <v>110</v>
+      </c>
+      <c r="I56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" s="2">
+        <v>42277.7732234259</v>
+      </c>
+      <c r="C57">
+        <v>5509650668</v>
+      </c>
+      <c r="F57" t="s">
         <v>62</v>
       </c>
-      <c r="C56">
-        <v>5509650478</v>
-      </c>
-      <c r="F56" t="s">
+      <c r="I57" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" s="2">
+        <v>42293.4550321991</v>
+      </c>
+      <c r="C58">
+        <v>5509650403</v>
+      </c>
+      <c r="D58">
+        <v>5509650460</v>
+      </c>
+      <c r="F58" t="s">
+        <v>63</v>
+      </c>
+      <c r="G58" t="s">
+        <v>106</v>
+      </c>
+      <c r="I58" t="s">
         <v>116</v>
       </c>
-      <c r="I56" t="s">
-        <v>169</v>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" s="2">
+        <v>42293.6616302431</v>
+      </c>
+      <c r="C59">
+        <v>5409650495</v>
+      </c>
+      <c r="D59">
+        <v>5409650305</v>
+      </c>
+      <c r="F59" t="s">
+        <v>64</v>
+      </c>
+      <c r="G59" t="s">
+        <v>107</v>
+      </c>
+      <c r="I59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" s="2">
+        <v>42272.5856828704</v>
+      </c>
+      <c r="C60">
+        <v>5309610078</v>
+      </c>
+      <c r="F60" t="s">
+        <v>65</v>
+      </c>
+      <c r="I60" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2164,13 +2543,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>183</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2178,10 +2557,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -2192,7 +2571,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>130</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2206,13 +2585,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2220,7 +2599,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2234,7 +2613,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2248,7 +2627,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2262,7 +2641,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2276,7 +2655,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2290,10 +2669,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -2304,7 +2683,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -2318,7 +2697,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="C12">
         <v>3</v>
@@ -2332,7 +2711,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -2346,7 +2725,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -2360,7 +2739,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -2374,7 +2753,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -2388,13 +2767,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2402,7 +2781,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -2416,13 +2795,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2430,7 +2809,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -2444,7 +2823,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>117</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2458,10 +2837,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -2472,13 +2851,732 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AR23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:44">
+      <c r="B1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I2" t="s">
+        <v>197</v>
+      </c>
+      <c r="K2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N2" t="s">
+        <v>203</v>
+      </c>
+      <c r="P2" t="s">
+        <v>217</v>
+      </c>
+      <c r="R2" t="s">
+        <v>225</v>
+      </c>
+      <c r="S2" t="s">
+        <v>235</v>
+      </c>
+      <c r="T2" t="s">
+        <v>239</v>
+      </c>
+      <c r="V2" t="s">
+        <v>189</v>
+      </c>
+      <c r="W2" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>252</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>235</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>199</v>
+      </c>
+      <c r="N3" t="s">
+        <v>204</v>
+      </c>
+      <c r="P3" t="s">
+        <v>218</v>
+      </c>
+      <c r="R3" t="s">
+        <v>226</v>
+      </c>
+      <c r="T3" t="s">
+        <v>240</v>
+      </c>
+      <c r="V3" t="s">
+        <v>240</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>253</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>204</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>205</v>
+      </c>
+      <c r="R4" t="s">
+        <v>205</v>
+      </c>
+      <c r="S4" t="s">
+        <v>205</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>205</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H5" t="s">
+        <v>190</v>
+      </c>
+      <c r="P5" t="s">
+        <v>190</v>
+      </c>
+      <c r="R5" t="s">
+        <v>179</v>
+      </c>
+      <c r="U5" t="s">
+        <v>244</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>191</v>
+      </c>
+      <c r="I6" t="s">
+        <v>191</v>
+      </c>
+      <c r="P6" t="s">
+        <v>219</v>
+      </c>
+      <c r="R6" t="s">
+        <v>219</v>
+      </c>
+      <c r="T6" t="s">
+        <v>241</v>
+      </c>
+      <c r="U6" t="s">
+        <v>241</v>
+      </c>
+      <c r="V6" t="s">
+        <v>246</v>
+      </c>
+      <c r="W6" t="s">
+        <v>191</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="V7" t="s">
+        <v>247</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>254</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="R8" t="s">
+        <v>227</v>
+      </c>
+      <c r="T8" t="s">
+        <v>227</v>
+      </c>
+      <c r="U8" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>227</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>206</v>
+      </c>
+      <c r="R9" t="s">
+        <v>206</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="N10" t="s">
+        <v>207</v>
+      </c>
+      <c r="P10" t="s">
+        <v>220</v>
+      </c>
+      <c r="S10" t="s">
+        <v>220</v>
+      </c>
+      <c r="V10" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>207</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>220</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>192</v>
+      </c>
+      <c r="N12" t="s">
+        <v>208</v>
+      </c>
+      <c r="O12" t="s">
+        <v>216</v>
+      </c>
+      <c r="R12" t="s">
+        <v>228</v>
+      </c>
+      <c r="T12" t="s">
+        <v>242</v>
+      </c>
+      <c r="V12" t="s">
+        <v>248</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>228</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>259</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>209</v>
+      </c>
+      <c r="R13" t="s">
+        <v>209</v>
+      </c>
+      <c r="T13" t="s">
+        <v>243</v>
+      </c>
+      <c r="V13" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>256</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>186</v>
+      </c>
+      <c r="N14" t="s">
+        <v>210</v>
+      </c>
+      <c r="R14" t="s">
+        <v>229</v>
+      </c>
+      <c r="S14" t="s">
+        <v>236</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>236</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>180</v>
+      </c>
+      <c r="P15" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>180</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H16" t="s">
+        <v>193</v>
+      </c>
+      <c r="J16" t="s">
+        <v>198</v>
+      </c>
+      <c r="N16" t="s">
+        <v>211</v>
+      </c>
+      <c r="P16" t="s">
+        <v>221</v>
+      </c>
+      <c r="R16" t="s">
+        <v>230</v>
+      </c>
+      <c r="S16" t="s">
+        <v>237</v>
+      </c>
+      <c r="T16" t="s">
+        <v>230</v>
+      </c>
+      <c r="V16" t="s">
+        <v>249</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>257</v>
+      </c>
+      <c r="AR16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:44">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>182</v>
+      </c>
+      <c r="P17" t="s">
+        <v>182</v>
+      </c>
+      <c r="S17" t="s">
+        <v>182</v>
+      </c>
+      <c r="T17" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>182</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:44">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>183</v>
+      </c>
+      <c r="N18" t="s">
+        <v>212</v>
+      </c>
+      <c r="R18" t="s">
+        <v>231</v>
+      </c>
+      <c r="S18" t="s">
+        <v>238</v>
+      </c>
+      <c r="U18" t="s">
+        <v>238</v>
+      </c>
+      <c r="V18" t="s">
+        <v>183</v>
+      </c>
+      <c r="AR18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:44">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>184</v>
+      </c>
+      <c r="H19" t="s">
+        <v>194</v>
+      </c>
+      <c r="K19" t="s">
+        <v>200</v>
+      </c>
+      <c r="N19" t="s">
+        <v>213</v>
+      </c>
+      <c r="P19" t="s">
+        <v>194</v>
+      </c>
+      <c r="R19" t="s">
+        <v>232</v>
+      </c>
+      <c r="T19" t="s">
+        <v>213</v>
+      </c>
+      <c r="U19" t="s">
+        <v>245</v>
+      </c>
+      <c r="V19" t="s">
+        <v>213</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>255</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>258</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>260</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>260</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>260</v>
+      </c>
+      <c r="AJ19" t="s">
+        <v>260</v>
+      </c>
+      <c r="AK19" t="s">
+        <v>260</v>
+      </c>
+      <c r="AR19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:44">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>195</v>
+      </c>
+      <c r="I20" t="s">
+        <v>195</v>
+      </c>
+      <c r="S20" t="s">
+        <v>195</v>
+      </c>
+      <c r="V20" t="s">
+        <v>195</v>
+      </c>
+      <c r="AR20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:44">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="P21" t="s">
+        <v>222</v>
+      </c>
+      <c r="AR21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:44">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>185</v>
+      </c>
+      <c r="H22" t="s">
+        <v>196</v>
+      </c>
+      <c r="M22" t="s">
+        <v>201</v>
+      </c>
+      <c r="N22" t="s">
+        <v>214</v>
+      </c>
+      <c r="P22" t="s">
+        <v>223</v>
+      </c>
+      <c r="R22" t="s">
+        <v>233</v>
+      </c>
+      <c r="S22" t="s">
+        <v>233</v>
+      </c>
+      <c r="T22" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>261</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:44">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="M23" t="s">
+        <v>202</v>
+      </c>
+      <c r="N23" t="s">
+        <v>215</v>
+      </c>
+      <c r="P23" t="s">
+        <v>224</v>
+      </c>
+      <c r="R23" t="s">
+        <v>234</v>
+      </c>
+      <c r="V23" t="s">
+        <v>250</v>
+      </c>
+      <c r="AR23" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>